<commit_message>
Added new agent functions
</commit_message>
<xml_diff>
--- a/HowToExcel/bin/Debug/netcoreapp3.1/Data.xlsx
+++ b/HowToExcel/bin/Debug/netcoreapp3.1/Data.xlsx
@@ -186,7 +186,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="0">
-        <v>20</v>
+        <v>300</v>
       </c>
       <c r="G2" s="0" t="s">
         <v>8</v>
@@ -209,7 +209,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="0">
-        <v>40</v>
+        <v>200</v>
       </c>
       <c r="G3" s="0" t="s">
         <v>10</v>
@@ -232,7 +232,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="0">
-        <v>20</v>
+        <v>2000</v>
       </c>
       <c r="G4" s="0" t="s">
         <v>12</v>
@@ -252,10 +252,10 @@
         <v>10</v>
       </c>
       <c r="C5" s="0">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5" s="0">
-        <v>20</v>
+        <v>400</v>
       </c>
       <c r="G5" s="0" t="s">
         <v>14</v>
@@ -278,7 +278,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="0">
-        <v>40</v>
+        <v>1700</v>
       </c>
       <c r="G6" s="0" t="s">
         <v>16</v>
@@ -301,7 +301,7 @@
         <v>5</v>
       </c>
       <c r="D7" s="0">
-        <v>20</v>
+        <v>1000</v>
       </c>
       <c r="G7" s="0" t="s">
         <v>18</v>
@@ -324,7 +324,7 @@
         <v>2</v>
       </c>
       <c r="D8" s="0">
-        <v>50</v>
+        <v>1200</v>
       </c>
       <c r="G8" s="0" t="s">
         <v>20</v>
@@ -347,7 +347,7 @@
         <v>4</v>
       </c>
       <c r="D9" s="0">
-        <v>40</v>
+        <v>600</v>
       </c>
       <c r="G9" s="0" t="s">
         <v>22</v>
@@ -370,7 +370,7 @@
         <v>3</v>
       </c>
       <c r="D10" s="0">
-        <v>30</v>
+        <v>400</v>
       </c>
       <c r="G10" s="0" t="s">
         <v>24</v>
@@ -393,7 +393,7 @@
         <v>4</v>
       </c>
       <c r="D11" s="0">
-        <v>30</v>
+        <v>300</v>
       </c>
       <c r="G11" s="0" t="s">
         <v>26</v>

</xml_diff>